<commit_message>
move main logistic to Account
</commit_message>
<xml_diff>
--- a/data/工具结息验算.xlsx
+++ b/data/工具结息验算.xlsx
@@ -422,16 +422,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2152650</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2238375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -449,7 +449,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5657850" y="2286000"/>
+          <a:off x="5267325" y="2143125"/>
           <a:ext cx="2438400" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
fix format and test data
</commit_message>
<xml_diff>
--- a/data/工具结息验算.xlsx
+++ b/data/工具结息验算.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>实际结息（透支解除）</t>
   </si>
@@ -51,7 +51,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>直接计算</t>
+    <t>换算成亿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接计算（单位：亿）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增利息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>误差</t>
+  </si>
+  <si>
+    <t>误差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>误差占比</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -59,11 +78,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.00000000%"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.0000000000_ ;_ * \-#,##0.0000000000_ ;_ * &quot;-&quot;??????????_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +103,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -150,19 +179,19 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -187,13 +216,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -234,13 +263,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>465931</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
@@ -281,13 +310,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -328,13 +357,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>571501</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -375,13 +404,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>581024</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>457199</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -402,7 +431,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11772899" y="1476375"/>
+          <a:off x="15649574" y="1476375"/>
           <a:ext cx="1933575" cy="295275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -757,22 +786,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="4" width="30.875" customWidth="1"/>
-    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.875" customWidth="1"/>
-    <col min="8" max="8" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -784,13 +814,22 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -798,25 +837,31 @@
         <v>2610694.2999999998</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <f>0.0261069444444*100000000</f>
         <v>2610694.4444399998</v>
       </c>
-      <c r="E2" s="6">
-        <f>B2+C2-D2</f>
+      <c r="E2" s="7">
+        <f t="shared" ref="E2:E5" si="0">B2+C2-I2</f>
         <v>-0.14443999994546175</v>
       </c>
       <c r="F2" s="5">
-        <f t="shared" ref="F2:F5" si="0">E2/D2</f>
+        <f t="shared" ref="F2:F5" si="1">E2/D2</f>
         <v>-5.5326275448693681E-8</v>
       </c>
-      <c r="G2" s="6">
-        <f>0.0261069444444*100000000</f>
+      <c r="G2" s="3">
+        <f>H2*100000000</f>
         <v>2610694.4444399998</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="6">
+        <v>2.6106944444399999E-2</v>
+      </c>
+      <c r="I2" s="3">
+        <f>G2</f>
+        <v>2610694.4444399998</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -824,27 +869,31 @@
         <v>4786249.7699999996</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <f>(0.0739694444444-0.0261069444444)*100000000</f>
         <v>4786250</v>
       </c>
-      <c r="E3" s="6">
-        <f t="shared" ref="E3:E6" si="1">B3+C3-D3</f>
+      <c r="E3" s="7">
+        <f t="shared" si="0"/>
         <v>-0.23000000044703484</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.8054322370756821E-8</v>
       </c>
-      <c r="G3" s="6">
-        <v>7394944.4400000004</v>
+      <c r="G3" s="3">
+        <f>H3*100000000</f>
+        <v>7396944.4444399998</v>
       </c>
       <c r="H3" s="6">
+        <v>7.3969444444399998E-2</v>
+      </c>
+      <c r="I3" s="3">
         <f>G3-G2</f>
-        <v>4784249.9955600007</v>
+        <v>4786250</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -852,27 +901,31 @@
         <v>8907777.4600000009</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <f>(0.163047222222-0.0739694444444)*100000000</f>
         <v>8907777.777759999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.31775999814271927</v>
+      </c>
+      <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>-0.31775999814271927</v>
-      </c>
-      <c r="F4" s="5">
-        <f t="shared" si="0"/>
         <v>-3.5672196373832869E-8</v>
       </c>
-      <c r="G4" s="6">
-        <v>16304722.220000001</v>
+      <c r="G4" s="3">
+        <f>H4*100000000</f>
+        <v>16304722.222199999</v>
       </c>
       <c r="H4" s="6">
-        <f>G4-G3</f>
-        <v>8909777.7800000012</v>
+        <v>0.16304722222199999</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I6" si="2">G4-G3</f>
+        <v>8907777.777759999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -882,27 +935,31 @@
       <c r="C5" s="2">
         <v>58500000</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <f>(0.845806944444-0.163047222222)*100000000</f>
         <v>68275972.222199991</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.31220000982284546</v>
+      </c>
+      <c r="F5" s="5">
         <f t="shared" si="1"/>
-        <v>-0.31219999492168427</v>
-      </c>
-      <c r="F5" s="5">
-        <f t="shared" si="0"/>
-        <v>-4.5726188109873912E-9</v>
-      </c>
-      <c r="G5" s="6">
-        <v>84580694.439999998</v>
+        <v>-4.5726190292363695E-9</v>
+      </c>
+      <c r="G5" s="3">
+        <f>H5*100000000</f>
+        <v>84580694.444399998</v>
       </c>
       <c r="H5" s="6">
-        <f>G5-G4</f>
-        <v>68275972.219999999</v>
+        <v>0.84580694444399995</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="2"/>
+        <v>68275972.222200006</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -912,27 +969,35 @@
       <c r="C6" s="2">
         <v>38250000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <f>(1.33399166667-0.845806944444)*100000000</f>
         <v>48818472.222600006</v>
       </c>
-      <c r="E6" s="7">
-        <f t="shared" si="1"/>
-        <v>-757638.59260000288</v>
+      <c r="E6" s="4">
+        <f>B6+C6-I6</f>
+        <v>-757638.59259999543</v>
       </c>
       <c r="F6" s="5">
-        <f>E6/G6</f>
-        <v>-5.6794851985412544E-3</v>
-      </c>
-      <c r="G6" s="6">
-        <v>133399166.67</v>
+        <f>E6/I6</f>
+        <v>-1.5519506410306192E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <f>H6*100000000</f>
+        <v>133399166.667</v>
       </c>
       <c r="H6" s="6">
-        <f>G6-G5</f>
-        <v>48818472.230000004</v>
+        <v>1.33399166667</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="2"/>
+        <v>48818472.222599998</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G7" s="3"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C17" t="s">
         <v>9</v>
       </c>
@@ -942,8 +1007,11 @@
       <c r="E17" t="s">
         <v>8</v>
       </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C18" s="3">
         <v>153941207.13870001</v>
       </c>
@@ -951,9 +1019,13 @@
         <f>1.57165694444*100000000</f>
         <v>157165694.44400001</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <f>C18-D18</f>
         <v>-3224487.3052999973</v>
+      </c>
+      <c r="F18">
+        <f>E18/C18</f>
+        <v>-2.0946225934130525E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>